<commit_message>
Enforce inform only queries
</commit_message>
<xml_diff>
--- a/backend/analysis/annotations/test_files/sample_1_SAF.xlsx
+++ b/backend/analysis/annotations/test_files/sample_1_SAF.xlsx
@@ -641,7 +641,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Ond,OndWB</t>
+          <t>OndWB</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -649,14 +649,9 @@
           <t>W</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>B,woordgroep(onderstrepen)</t>
-        </is>
-      </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>I,I,I,III</t>
+          <t>I,III</t>
         </is>
       </c>
     </row>
@@ -810,7 +805,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Ond,OndWB,Sz2+</t>
+          <t>OndWB</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -818,39 +813,14 @@
           <t>W</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Ond,woordgroep(onderstrepen)</t>
-        </is>
-      </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>W,Werkwoordswoordgroep</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>B,Ond</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>B</t>
+          <t>W</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>I,I,I,I,I,I,I,I,I,III,III</t>
+          <t>I,I,III</t>
         </is>
       </c>
     </row>
@@ -977,32 +947,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>B,Inv,OndWBB,OndWBVC</t>
+          <t>Inv,OndWBB,OndWBVC</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>W,Werkwoordswoordgroep</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Ond</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>VC</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>B</t>
+          <t>W</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>I,I,I,I,III,III,IV,IV</t>
+          <t>I,III,IV,IV</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1080,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Ond,OndWBB</t>
+          <t>OndWBB</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1133,19 +1088,9 @@
           <t>W</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>I,I,I,I,IV</t>
+          <t>I,IV</t>
         </is>
       </c>
     </row>
@@ -1264,7 +1209,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Ond,OndWB</t>
+          <t>OndWB</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1272,14 +1217,9 @@
           <t>W</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>B,woordgroep(onderstrepen)</t>
-        </is>
-      </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>I,I,I,III</t>
+          <t>I,III</t>
         </is>
       </c>
     </row>
@@ -1415,7 +1355,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Ond,OndWBB,Sz2+</t>
+          <t>OndWBB</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1423,29 +1363,14 @@
           <t>W</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>B,woordgroep(onderstrepen)</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
       <c r="H37" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>VC</t>
-        </is>
-      </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>I,I,I,I,I,IV</t>
+          <t>I,I,IV</t>
         </is>
       </c>
     </row>
@@ -1551,16 +1476,6 @@
           <t>Zc</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>PV-loos</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>B,woordgroep(onderstrepen)</t>
-        </is>
-      </c>
       <c r="G42" t="inlineStr">
         <is>
           <t>W</t>
@@ -1568,7 +1483,7 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>I,I</t>
+          <t>I</t>
         </is>
       </c>
     </row>
@@ -1705,7 +1620,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Ond,OndWBVC</t>
+          <t>OndWBVC</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1713,19 +1628,9 @@
           <t>W</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>VC</t>
-        </is>
-      </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>I,I,I,IV</t>
+          <t>I,IV</t>
         </is>
       </c>
     </row>
@@ -1858,21 +1763,6 @@
           <t>Zc</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>B,woordgroep(onderstrepen)</t>
-        </is>
-      </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>woordgroep(onderstrepen)</t>
-        </is>
-      </c>
-      <c r="N53" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -1885,7 +1775,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>B,Inv,OndWB</t>
+          <t>Inv,OndWB</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1893,14 +1783,9 @@
           <t>W</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>Ond</t>
-        </is>
-      </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>I,I,I,III,III</t>
+          <t>I,III,III</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjust safreader test to new sastadev
</commit_message>
<xml_diff>
--- a/backend/analysis/annotations/test_files/sample_1_SAF.xlsx
+++ b/backend/analysis/annotations/test_files/sample_1_SAF.xlsx
@@ -528,7 +528,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
@@ -567,7 +567,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -577,7 +577,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -597,7 +597,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -622,7 +622,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -632,7 +632,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -657,7 +657,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
@@ -716,7 +716,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -726,7 +726,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -746,7 +746,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -786,7 +786,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -796,7 +796,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -831,7 +831,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
@@ -878,7 +878,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -888,7 +888,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -908,7 +908,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -933,7 +933,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -943,7 +943,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -968,7 +968,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1150,7 +1150,7 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1170,7 +1170,7 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1230,7 +1230,7 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1291,7 +1291,7 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1341,7 +1341,7 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1454,7 +1454,7 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1474,7 +1474,7 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
@@ -1541,7 +1541,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -1676,7 +1676,7 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -1701,7 +1701,7 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -1741,7 +1741,7 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>

</xml_diff>